<commit_message>
add graph image to excell report
</commit_message>
<xml_diff>
--- a/Reports/Drift_Check.xlsx
+++ b/Reports/Drift_Check.xlsx
@@ -122,6 +122,36 @@
     </indexedColors>
   </colors>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>4</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3638550" cy="2533650"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -457,10 +487,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.000276</v>
+        <v>0.001356</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>0.001303</v>
       </c>
     </row>
     <row r="3">
@@ -470,10 +500,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.00015</v>
+        <v>0.000645</v>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>0.000688</v>
       </c>
     </row>
     <row r="4">
@@ -483,10 +513,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.00036</v>
+        <v>0.001835</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>0.001573</v>
       </c>
     </row>
     <row r="5">
@@ -496,10 +526,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.000388</v>
+        <v>0.002054</v>
       </c>
       <c r="C5" t="n">
-        <v>0.000175</v>
+        <v>0.001809</v>
       </c>
     </row>
     <row r="6">
@@ -509,10 +539,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.000472</v>
+        <v>0.003406</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>0.002288</v>
       </c>
     </row>
     <row r="7">
@@ -522,10 +552,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.000462</v>
+        <v>0.003855</v>
       </c>
       <c r="C7" t="n">
-        <v>0</v>
+        <v>0.002674</v>
       </c>
     </row>
   </sheetData>
@@ -542,8 +572,9 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
limit of displacement is accurated and ui window designed better
</commit_message>
<xml_diff>
--- a/Reports/Drift_Check.xlsx
+++ b/Reports/Drift_Check.xlsx
@@ -483,27 +483,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>B1</t>
+          <t>B2</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.000276</v>
+        <v>0.000322</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>0.000344</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>B2</t>
+          <t>B1</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.00015</v>
+        <v>0.000678</v>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>0.000652</v>
       </c>
     </row>
     <row r="4">
@@ -513,10 +513,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.00036</v>
+        <v>0.000918</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>0.000787</v>
       </c>
     </row>
     <row r="5">
@@ -526,10 +526,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.000388</v>
+        <v>0.001027</v>
       </c>
       <c r="C5" t="n">
-        <v>0.000175</v>
+        <v>0.000905</v>
       </c>
     </row>
     <row r="6">
@@ -539,10 +539,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.000472</v>
+        <v>0.001703</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>0.001144</v>
       </c>
     </row>
     <row r="7">
@@ -552,10 +552,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.000462</v>
+        <v>0.001928</v>
       </c>
       <c r="C7" t="n">
-        <v>0</v>
+        <v>0.001337</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
last msg for max drift is changed to drift and displacement which one was active
</commit_message>
<xml_diff>
--- a/Reports/Drift_Check.xlsx
+++ b/Reports/Drift_Check.xlsx
@@ -487,10 +487,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.000322</v>
+        <v>0.000877</v>
       </c>
       <c r="C2" t="n">
-        <v>0.000344</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -500,10 +500,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.000678</v>
+        <v>0.002698</v>
       </c>
       <c r="C3" t="n">
-        <v>0.000652</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -513,10 +513,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.000918</v>
+        <v>0.006253</v>
       </c>
       <c r="C4" t="n">
-        <v>0.000787</v>
+        <v>0.002547</v>
       </c>
     </row>
     <row r="5">
@@ -526,10 +526,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.001027</v>
+        <v>0.00937</v>
       </c>
       <c r="C5" t="n">
-        <v>0.000905</v>
+        <v>0.003992</v>
       </c>
     </row>
     <row r="6">
@@ -539,10 +539,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.001703</v>
+        <v>0.013521</v>
       </c>
       <c r="C6" t="n">
-        <v>0.001144</v>
+        <v>0.005641</v>
       </c>
     </row>
     <row r="7">
@@ -552,10 +552,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.001928</v>
+        <v>0.018716</v>
       </c>
       <c r="C7" t="n">
-        <v>0.001337</v>
+        <v>0.008170999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
some edit to wellcome window witch work correctly
</commit_message>
<xml_diff>
--- a/Reports/Drift_Check.xlsx
+++ b/Reports/Drift_Check.xlsx
@@ -487,7 +487,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.000419</v>
+        <v>0.00015</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
@@ -500,7 +500,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.001179</v>
+        <v>0.000276</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
@@ -513,7 +513,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.002588</v>
+        <v>0.00036</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
@@ -526,10 +526,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.003772</v>
+        <v>0.000388</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>0.000175</v>
       </c>
     </row>
     <row r="6">
@@ -539,7 +539,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.005137</v>
+        <v>0.000472</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
@@ -552,7 +552,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.006615</v>
+        <v>0.000462</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
change to 2 window with new colors and new stype, inverse data table, add basement elevt to table and graph, pointpan som buttons and list, omit index of table
</commit_message>
<xml_diff>
--- a/Reports/Drift_Check.xlsx
+++ b/Reports/Drift_Check.xlsx
@@ -133,7 +133,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="3638550" cy="3486150"/>
+    <ext cx="3714750" cy="3514725"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -155,8 +155,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C7" headerRowCount="1">
-  <autoFilter ref="A1:C7"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C8" headerRowCount="1">
+  <autoFilter ref="A1:C8"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Story"/>
     <tableColumn id="2" name="X"/>
@@ -455,7 +455,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -483,11 +483,11 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>B2</t>
+          <t>Bs</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.00015</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
@@ -496,11 +496,11 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>B1</t>
+          <t>B2</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.000276</v>
+        <v>0.00015</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
@@ -509,11 +509,11 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>G</t>
+          <t>B1</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.00036</v>
+        <v>0.000276</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
@@ -522,44 +522,57 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>L1</t>
+          <t>G</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.000388</v>
+        <v>0.00036</v>
       </c>
       <c r="C5" t="n">
-        <v>0.000175</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>L2</t>
+          <t>L1</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.000472</v>
+        <v>0.000388</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>0.000175</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>L2</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0.000472</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
           <t>L3</t>
         </is>
       </c>
-      <c r="B7" t="n">
+      <c r="B8" t="n">
         <v>0.000462</v>
       </c>
-      <c r="C7" t="n">
+      <c r="C8" t="n">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:C7">
+  <conditionalFormatting sqref="A1:C8">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="num" val="0.002"/>

</xml_diff>

<commit_message>
manage run and drift button and manage open file and connect button.
</commit_message>
<xml_diff>
--- a/Reports/Drift_Check.xlsx
+++ b/Reports/Drift_Check.xlsx
@@ -133,7 +133,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="3714750" cy="3514725"/>
+    <ext cx="4191000" cy="3514725"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -500,7 +500,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.00015</v>
+        <v>0.016486</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
@@ -513,7 +513,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.000276</v>
+        <v>0.046425</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
@@ -526,7 +526,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.00036</v>
+        <v>0.101896</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
@@ -539,10 +539,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.000388</v>
+        <v>0.148517</v>
       </c>
       <c r="C6" t="n">
-        <v>0.000175</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -552,7 +552,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.000472</v>
+        <v>0.202233</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
@@ -565,7 +565,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.000462</v>
+        <v>0.260445</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>

</xml_diff>